<commit_message>
updated info with Mazarrasa study published
</commit_message>
<xml_diff>
--- a/data_paper/studies/studies_edited.xlsx
+++ b/data_paper/studies/studies_edited.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofcambridgecloud-my.sharepoint.com/personal/tlgm2_cam_ac_uk/Documents/Documents/07_Cam_postdoc/SaltmarshC/data_paper/studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:40009_{85CC4C6B-8A06-482E-821A-15A51B4154D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07F2932C-84B9-474C-BADA-538AE3220CDE}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:40009_{85CC4C6B-8A06-482E-821A-15A51B4154D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A72C1EF-4B10-44B6-91CA-0E516012EC71}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="studies_edited" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,13 @@
   </definedNames>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="121">
   <si>
     <t>Data_type</t>
   </si>
@@ -384,6 +384,12 @@
   </si>
   <si>
     <t>Review</t>
+  </si>
+  <si>
+    <t>Mazarrasa et al 2023</t>
+  </si>
+  <si>
+    <t>Hatje et al 2023</t>
   </si>
 </sst>
 </file>
@@ -943,9 +949,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Tania" refreshedDate="44988.505510416668" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="97" xr:uid="{B886DFCD-5F8E-4101-B228-E3DF37679AF1}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Tania" refreshedDate="45084.703390625" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="99" xr:uid="{0C86014F-C8AF-4AF6-9D46-6315065C5E04}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:D99" sheet="studies_edited"/>
+    <worksheetSource ref="A1:D100" sheet="studies_edited"/>
   </cacheSource>
   <cacheFields count="4">
     <cacheField name="Data_type" numFmtId="0">
@@ -980,7 +986,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="97">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="99">
   <r>
     <s v="Core-level"/>
     <s v="Adame et al 2013"/>
@@ -1181,9 +1187,9 @@
   </r>
   <r>
     <s v="Core-level"/>
-    <s v="Mazarrasa et al in prep"/>
+    <s v="Mazarrasa et al 2023"/>
     <n v="413"/>
-    <x v="6"/>
+    <x v="0"/>
   </r>
   <r>
     <s v="Core-level"/>
@@ -1229,6 +1235,12 @@
   </r>
   <r>
     <s v="Core-level"/>
+    <s v="Russell et al submitted"/>
+    <n v="253"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <s v="Core-level"/>
     <s v="Sammul et al 2012"/>
     <n v="41"/>
     <x v="3"/>
@@ -1336,31 +1348,31 @@
     <x v="5"/>
   </r>
   <r>
-    <s v="Meta-analysis"/>
-    <s v="Copertino et al under review"/>
-    <n v="251"/>
-    <x v="6"/>
-  </r>
-  <r>
-    <s v="Meta-analysis"/>
+    <s v="Review"/>
     <s v="Fu et al 2021"/>
     <n v="8"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="Meta-analysis"/>
+    <s v="Review"/>
+    <s v="Hatje et al 2023"/>
+    <n v="251"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="Review"/>
     <s v="He et al 2020"/>
     <n v="43"/>
     <x v="7"/>
   </r>
   <r>
-    <s v="Meta-analysis"/>
+    <s v="Review"/>
     <s v="Hu et al 2020"/>
     <n v="187"/>
     <x v="3"/>
   </r>
   <r>
-    <s v="Meta-analysis"/>
+    <s v="Review"/>
     <s v="Wails et al 2021"/>
     <n v="2"/>
     <x v="7"/>
@@ -1373,6 +1385,12 @@
   </r>
   <r>
     <s v="Site-level"/>
+    <s v="Ferronato et al 2019"/>
+    <n v="27"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="Site-level"/>
     <s v="Gailis et al 2021"/>
     <n v="22"/>
     <x v="2"/>
@@ -1567,7 +1585,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{03A893EB-397C-4C72-ADD2-5E0C08D7E60A}" name="PivotTable6" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5D5D7A9-2919-450E-BC09-C87947A59A57}" name="PivotTable6" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F2:G12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -1940,8 +1958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2093,7 +2111,7 @@
         <v>82</v>
       </c>
       <c r="G4" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2113,7 +2131,7 @@
         <v>88</v>
       </c>
       <c r="G5" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2153,7 +2171,7 @@
         <v>84</v>
       </c>
       <c r="G7" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2253,7 +2271,7 @@
         <v>91</v>
       </c>
       <c r="G12" s="4">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2568,14 +2586,14 @@
       <c r="A35" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>37</v>
+      <c r="B35" t="s">
+        <v>119</v>
       </c>
       <c r="C35" s="1">
         <v>413</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2687,7 +2705,7 @@
         <v>253</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2947,27 +2965,27 @@
         <v>118</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C62" s="1">
-        <v>251</v>
+        <v>8</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>118</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>65</v>
+      <c r="B63" t="s">
+        <v>120</v>
       </c>
       <c r="C63" s="1">
-        <v>8</v>
+        <v>251</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>